<commit_message>
feat: generate Excel report for reorder strategy recommendations
</commit_message>
<xml_diff>
--- a/backend/charts/reorder/optimization_recommendations.xlsx
+++ b/backend/charts/reorder/optimization_recommendations.xlsx
@@ -17,13 +17,16 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -34,7 +37,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -42,12 +45,21 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -413,14 +425,106 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>category</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>recommendation</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>new_safety_stock</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>new_reorder_point</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>new_optimal_inventory</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>new_holding_cost</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>potential_saving</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>toys</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Giảm Safety Stock từ 93263 → 74610 và Reorder Point từ 507836 → 457052 để tiết kiệm chi phí.</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>74610</v>
+      </c>
+      <c r="D2" t="n">
+        <v>457052</v>
+      </c>
+      <c r="E2" t="n">
+        <v>531662</v>
+      </c>
+      <c r="F2" t="n">
+        <v>1169656</v>
+      </c>
+      <c r="G2" t="n">
+        <v>-640689</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>garden_tools</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Giảm Safety Stock từ 1552 → 1241 và Reorder Point từ 189523 → 170570 để tiết kiệm chi phí.</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>1241</v>
+      </c>
+      <c r="D3" t="n">
+        <v>170570</v>
+      </c>
+      <c r="E3" t="n">
+        <v>171811</v>
+      </c>
+      <c r="F3" t="n">
+        <v>412346</v>
+      </c>
+      <c r="G3" t="n">
+        <v>-228914</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fix: currency formatting to convert BRL to VND in charts
</commit_message>
<xml_diff>
--- a/backend/charts/reorder/optimization_recommendations.xlsx
+++ b/backend/charts/reorder/optimization_recommendations.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -473,55 +473,271 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>toys</t>
+          <t>garden_tools</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Giảm Safety Stock từ 93263 → 74610 và Reorder Point từ 507836 → 457052 để tiết kiệm chi phí.</t>
+          <t>Giảm Safety Stock từ 1552 → 1241 và Reorder Point từ 189523 → 170570 để tiết kiệm chi phí.</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>74610</v>
+        <v>1241</v>
       </c>
       <c r="D2" t="n">
-        <v>457052</v>
+        <v>170570</v>
       </c>
       <c r="E2" t="n">
-        <v>531662</v>
+        <v>171811</v>
       </c>
       <c r="F2" t="n">
-        <v>1169656</v>
+        <v>2144201280</v>
       </c>
       <c r="G2" t="n">
-        <v>-640689</v>
+        <v>-1190354880</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>garden_tools</t>
+          <t>watches_gifts</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Giảm Safety Stock từ 1552 → 1241 và Reorder Point từ 189523 → 170570 để tiết kiệm chi phí.</t>
+          <t>Giảm Safety Stock từ 501 → 400 và Reorder Point từ 40167 → 36150 để tiết kiệm chi phí.</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>1241</v>
+        <v>400</v>
       </c>
       <c r="D3" t="n">
-        <v>170570</v>
+        <v>36150</v>
       </c>
       <c r="E3" t="n">
-        <v>171811</v>
+        <v>36550</v>
       </c>
       <c r="F3" t="n">
-        <v>412346</v>
+        <v>427635000</v>
       </c>
       <c r="G3" t="n">
-        <v>-228914</v>
+        <v>-237308760</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>furniture_decor</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Giảm Safety Stock từ 550 → 440 và Reorder Point từ 8075 → 7267 để tiết kiệm chi phí.</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>440</v>
+      </c>
+      <c r="D4" t="n">
+        <v>7267</v>
+      </c>
+      <c r="E4" t="n">
+        <v>7707</v>
+      </c>
+      <c r="F4" t="n">
+        <v>78148980</v>
+      </c>
+      <c r="G4" t="n">
+        <v>-43165980</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>bed_bath_table</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Giảm Safety Stock từ 146 → 116 và Reorder Point từ 7536 → 6782 để tiết kiệm chi phí.</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>116</v>
+      </c>
+      <c r="D5" t="n">
+        <v>6782</v>
+      </c>
+      <c r="E5" t="n">
+        <v>6898</v>
+      </c>
+      <c r="F5" t="n">
+        <v>71739200</v>
+      </c>
+      <c r="G5" t="n">
+        <v>-39782080</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>electronics</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Giảm Safety Stock từ 152 → 121 và Reorder Point từ 6341 → 5706 để tiết kiệm chi phí.</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>121</v>
+      </c>
+      <c r="D6" t="n">
+        <v>5706</v>
+      </c>
+      <c r="E6" t="n">
+        <v>5827</v>
+      </c>
+      <c r="F6" t="n">
+        <v>59085780</v>
+      </c>
+      <c r="G6" t="n">
+        <v>-32750172</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>auto</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Giảm Safety Stock từ 70 → 56 và Reorder Point từ 5684 → 5115 để tiết kiệm chi phí.</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>56</v>
+      </c>
+      <c r="D7" t="n">
+        <v>5115</v>
+      </c>
+      <c r="E7" t="n">
+        <v>5171</v>
+      </c>
+      <c r="F7" t="n">
+        <v>44367180</v>
+      </c>
+      <c r="G7" t="n">
+        <v>-24619452</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>sports_leisure</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Giảm Safety Stock từ 894 → 715 và Reorder Point từ 3548 → 3193 để tiết kiệm chi phí.</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>715</v>
+      </c>
+      <c r="D8" t="n">
+        <v>3193</v>
+      </c>
+      <c r="E8" t="n">
+        <v>3908</v>
+      </c>
+      <c r="F8" t="n">
+        <v>38611040</v>
+      </c>
+      <c r="G8" t="n">
+        <v>-21056256</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>baby</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Giảm Safety Stock từ 0 → 0 và Reorder Point từ 3749 → 3374 để tiết kiệm chi phí.</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>0</v>
+      </c>
+      <c r="D9" t="n">
+        <v>3374</v>
+      </c>
+      <c r="E9" t="n">
+        <v>3374</v>
+      </c>
+      <c r="F9" t="n">
+        <v>32457880</v>
+      </c>
+      <c r="G9" t="n">
+        <v>-18031728</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>health_beauty</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Giảm Safety Stock từ 283 → 226 và Reorder Point từ 2317 → 2085 để tiết kiệm chi phí.</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>226</v>
+      </c>
+      <c r="D10" t="n">
+        <v>2085</v>
+      </c>
+      <c r="E10" t="n">
+        <v>2311</v>
+      </c>
+      <c r="F10" t="n">
+        <v>22231820</v>
+      </c>
+      <c r="G10" t="n">
+        <v>-12227020</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>construction_tools_construction</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Giảm Safety Stock từ 0 → 0 và Reorder Point từ 2035 → 1831 để tiết kiệm chi phí.</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>0</v>
+      </c>
+      <c r="D11" t="n">
+        <v>1831</v>
+      </c>
+      <c r="E11" t="n">
+        <v>1831</v>
+      </c>
+      <c r="F11" t="n">
+        <v>15233920</v>
+      </c>
+      <c r="G11" t="n">
+        <v>-8461440</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat(database): Integrate MongoDB Atlas for persistent data storage
</commit_message>
<xml_diff>
--- a/backend/charts/reorder/optimization_recommendations.xlsx
+++ b/backend/charts/reorder/optimization_recommendations.xlsx
@@ -16,7 +16,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
+  </numFmts>
   <fonts count="2">
     <font>
       <name val="Calibri"/>
@@ -55,11 +58,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -425,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -469,6 +473,11 @@
           <t>potential_saving</t>
         </is>
       </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>timestamp</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -496,6 +505,9 @@
       <c r="G2" t="n">
         <v>-1190354880</v>
       </c>
+      <c r="H2" s="2" t="n">
+        <v>45764.31028708907</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -523,6 +535,9 @@
       <c r="G3" t="n">
         <v>-237308760</v>
       </c>
+      <c r="H3" s="2" t="n">
+        <v>45764.31028708907</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -550,6 +565,9 @@
       <c r="G4" t="n">
         <v>-43165980</v>
       </c>
+      <c r="H4" s="2" t="n">
+        <v>45764.31028708907</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -577,6 +595,9 @@
       <c r="G5" t="n">
         <v>-39782080</v>
       </c>
+      <c r="H5" s="2" t="n">
+        <v>45764.31028708907</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -604,6 +625,9 @@
       <c r="G6" t="n">
         <v>-32750172</v>
       </c>
+      <c r="H6" s="2" t="n">
+        <v>45764.31028708907</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -631,6 +655,9 @@
       <c r="G7" t="n">
         <v>-24619452</v>
       </c>
+      <c r="H7" s="2" t="n">
+        <v>45764.31028708907</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -658,6 +685,9 @@
       <c r="G8" t="n">
         <v>-21056256</v>
       </c>
+      <c r="H8" s="2" t="n">
+        <v>45764.31028708907</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -685,6 +715,9 @@
       <c r="G9" t="n">
         <v>-18031728</v>
       </c>
+      <c r="H9" s="2" t="n">
+        <v>45764.31028708907</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -712,6 +745,9 @@
       <c r="G10" t="n">
         <v>-12227020</v>
       </c>
+      <c r="H10" s="2" t="n">
+        <v>45764.31028708907</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -738,6 +774,9 @@
       </c>
       <c r="G11" t="n">
         <v>-8461440</v>
+      </c>
+      <c r="H11" s="2" t="n">
+        <v>45764.31028708907</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: optimize data processing with Spark and integrate with NumPy & Pandas
</commit_message>
<xml_diff>
--- a/backend/charts/reorder/optimization_recommendations.xlsx
+++ b/backend/charts/reorder/optimization_recommendations.xlsx
@@ -506,7 +506,7 @@
         <v>-1190354880</v>
       </c>
       <c r="H2" s="2" t="n">
-        <v>45764.31028708907</v>
+        <v>45765.24092908231</v>
       </c>
     </row>
     <row r="3">
@@ -536,7 +536,7 @@
         <v>-237308760</v>
       </c>
       <c r="H3" s="2" t="n">
-        <v>45764.31028708907</v>
+        <v>45765.24092908231</v>
       </c>
     </row>
     <row r="4">
@@ -566,7 +566,7 @@
         <v>-43165980</v>
       </c>
       <c r="H4" s="2" t="n">
-        <v>45764.31028708907</v>
+        <v>45765.24092908231</v>
       </c>
     </row>
     <row r="5">
@@ -596,7 +596,7 @@
         <v>-39782080</v>
       </c>
       <c r="H5" s="2" t="n">
-        <v>45764.31028708907</v>
+        <v>45765.24092908231</v>
       </c>
     </row>
     <row r="6">
@@ -626,7 +626,7 @@
         <v>-32750172</v>
       </c>
       <c r="H6" s="2" t="n">
-        <v>45764.31028708907</v>
+        <v>45765.24092908231</v>
       </c>
     </row>
     <row r="7">
@@ -656,7 +656,7 @@
         <v>-24619452</v>
       </c>
       <c r="H7" s="2" t="n">
-        <v>45764.31028708907</v>
+        <v>45765.24092908231</v>
       </c>
     </row>
     <row r="8">
@@ -686,7 +686,7 @@
         <v>-21056256</v>
       </c>
       <c r="H8" s="2" t="n">
-        <v>45764.31028708907</v>
+        <v>45765.24092908231</v>
       </c>
     </row>
     <row r="9">
@@ -716,7 +716,7 @@
         <v>-18031728</v>
       </c>
       <c r="H9" s="2" t="n">
-        <v>45764.31028708907</v>
+        <v>45765.24092908231</v>
       </c>
     </row>
     <row r="10">
@@ -746,7 +746,7 @@
         <v>-12227020</v>
       </c>
       <c r="H10" s="2" t="n">
-        <v>45764.31028708907</v>
+        <v>45765.24092908231</v>
       </c>
     </row>
     <row r="11">
@@ -776,7 +776,7 @@
         <v>-8461440</v>
       </c>
       <c r="H11" s="2" t="n">
-        <v>45764.31028708907</v>
+        <v>45765.24092908231</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
docs: add initial README
</commit_message>
<xml_diff>
--- a/backend/charts/reorder/optimization_recommendations.xlsx
+++ b/backend/charts/reorder/optimization_recommendations.xlsx
@@ -506,7 +506,7 @@
         <v>-1190354880</v>
       </c>
       <c r="H2" s="2" t="n">
-        <v>45765.24092908231</v>
+        <v>45767.431891083</v>
       </c>
     </row>
     <row r="3">
@@ -536,7 +536,7 @@
         <v>-237308760</v>
       </c>
       <c r="H3" s="2" t="n">
-        <v>45765.24092908231</v>
+        <v>45767.431891083</v>
       </c>
     </row>
     <row r="4">
@@ -566,7 +566,7 @@
         <v>-43165980</v>
       </c>
       <c r="H4" s="2" t="n">
-        <v>45765.24092908231</v>
+        <v>45767.431891083</v>
       </c>
     </row>
     <row r="5">
@@ -596,7 +596,7 @@
         <v>-39782080</v>
       </c>
       <c r="H5" s="2" t="n">
-        <v>45765.24092908231</v>
+        <v>45767.431891083</v>
       </c>
     </row>
     <row r="6">
@@ -626,7 +626,7 @@
         <v>-32750172</v>
       </c>
       <c r="H6" s="2" t="n">
-        <v>45765.24092908231</v>
+        <v>45767.431891083</v>
       </c>
     </row>
     <row r="7">
@@ -656,7 +656,7 @@
         <v>-24619452</v>
       </c>
       <c r="H7" s="2" t="n">
-        <v>45765.24092908231</v>
+        <v>45767.431891083</v>
       </c>
     </row>
     <row r="8">
@@ -686,7 +686,7 @@
         <v>-21056256</v>
       </c>
       <c r="H8" s="2" t="n">
-        <v>45765.24092908231</v>
+        <v>45767.431891083</v>
       </c>
     </row>
     <row r="9">
@@ -716,7 +716,7 @@
         <v>-18031728</v>
       </c>
       <c r="H9" s="2" t="n">
-        <v>45765.24092908231</v>
+        <v>45767.431891083</v>
       </c>
     </row>
     <row r="10">
@@ -746,7 +746,7 @@
         <v>-12227020</v>
       </c>
       <c r="H10" s="2" t="n">
-        <v>45765.24092908231</v>
+        <v>45767.431891083</v>
       </c>
     </row>
     <row r="11">
@@ -776,7 +776,7 @@
         <v>-8461440</v>
       </c>
       <c r="H11" s="2" t="n">
-        <v>45765.24092908231</v>
+        <v>45767.431891083</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
refactor: rename text and identifiers
</commit_message>
<xml_diff>
--- a/backend/charts/reorder/optimization_recommendations.xlsx
+++ b/backend/charts/reorder/optimization_recommendations.xlsx
@@ -487,7 +487,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Giảm Safety Stock từ 1552 → 1241 và Reorder Point từ 189523 → 170570 để tiết kiệm chi phí.</t>
+          <t>Reduce Safety Stock from 1552 → 1241 and Reorder Point from 189523 → 170570 to save costs.</t>
         </is>
       </c>
       <c r="C2" t="n">
@@ -506,7 +506,7 @@
         <v>-1190354880</v>
       </c>
       <c r="H2" s="2" t="n">
-        <v>45767.431891083</v>
+        <v>45786.07619457495</v>
       </c>
     </row>
     <row r="3">
@@ -517,7 +517,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Giảm Safety Stock từ 501 → 400 và Reorder Point từ 40167 → 36150 để tiết kiệm chi phí.</t>
+          <t>Reduce Safety Stock from 501 → 400 and Reorder Point from 40167 → 36150 to save costs.</t>
         </is>
       </c>
       <c r="C3" t="n">
@@ -536,7 +536,7 @@
         <v>-237308760</v>
       </c>
       <c r="H3" s="2" t="n">
-        <v>45767.431891083</v>
+        <v>45786.07619457495</v>
       </c>
     </row>
     <row r="4">
@@ -547,7 +547,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Giảm Safety Stock từ 550 → 440 và Reorder Point từ 8075 → 7267 để tiết kiệm chi phí.</t>
+          <t>Reduce Safety Stock from 550 → 440 and Reorder Point from 8075 → 7267 to save costs.</t>
         </is>
       </c>
       <c r="C4" t="n">
@@ -566,7 +566,7 @@
         <v>-43165980</v>
       </c>
       <c r="H4" s="2" t="n">
-        <v>45767.431891083</v>
+        <v>45786.07619457495</v>
       </c>
     </row>
     <row r="5">
@@ -577,7 +577,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Giảm Safety Stock từ 146 → 116 và Reorder Point từ 7536 → 6782 để tiết kiệm chi phí.</t>
+          <t>Reduce Safety Stock from 146 → 116 and Reorder Point from 7536 → 6782 to save costs.</t>
         </is>
       </c>
       <c r="C5" t="n">
@@ -596,7 +596,7 @@
         <v>-39782080</v>
       </c>
       <c r="H5" s="2" t="n">
-        <v>45767.431891083</v>
+        <v>45786.07619457495</v>
       </c>
     </row>
     <row r="6">
@@ -607,7 +607,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Giảm Safety Stock từ 152 → 121 và Reorder Point từ 6341 → 5706 để tiết kiệm chi phí.</t>
+          <t>Reduce Safety Stock from 152 → 121 and Reorder Point from 6341 → 5706 to save costs.</t>
         </is>
       </c>
       <c r="C6" t="n">
@@ -626,7 +626,7 @@
         <v>-32750172</v>
       </c>
       <c r="H6" s="2" t="n">
-        <v>45767.431891083</v>
+        <v>45786.07619457495</v>
       </c>
     </row>
     <row r="7">
@@ -637,7 +637,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Giảm Safety Stock từ 70 → 56 và Reorder Point từ 5684 → 5115 để tiết kiệm chi phí.</t>
+          <t>Reduce Safety Stock from 70 → 56 and Reorder Point from 5684 → 5115 to save costs.</t>
         </is>
       </c>
       <c r="C7" t="n">
@@ -656,7 +656,7 @@
         <v>-24619452</v>
       </c>
       <c r="H7" s="2" t="n">
-        <v>45767.431891083</v>
+        <v>45786.07619457495</v>
       </c>
     </row>
     <row r="8">
@@ -667,7 +667,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Giảm Safety Stock từ 894 → 715 và Reorder Point từ 3548 → 3193 để tiết kiệm chi phí.</t>
+          <t>Reduce Safety Stock from 894 → 715 and Reorder Point from 3548 → 3193 to save costs.</t>
         </is>
       </c>
       <c r="C8" t="n">
@@ -686,7 +686,7 @@
         <v>-21056256</v>
       </c>
       <c r="H8" s="2" t="n">
-        <v>45767.431891083</v>
+        <v>45786.07619457495</v>
       </c>
     </row>
     <row r="9">
@@ -697,7 +697,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Giảm Safety Stock từ 0 → 0 và Reorder Point từ 3749 → 3374 để tiết kiệm chi phí.</t>
+          <t>Reduce Safety Stock from 0 → 0 and Reorder Point from 3749 → 3374 to save costs.</t>
         </is>
       </c>
       <c r="C9" t="n">
@@ -716,7 +716,7 @@
         <v>-18031728</v>
       </c>
       <c r="H9" s="2" t="n">
-        <v>45767.431891083</v>
+        <v>45786.07619457495</v>
       </c>
     </row>
     <row r="10">
@@ -727,7 +727,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Giảm Safety Stock từ 283 → 226 và Reorder Point từ 2317 → 2085 để tiết kiệm chi phí.</t>
+          <t>Reduce Safety Stock from 283 → 226 and Reorder Point from 2317 → 2085 to save costs.</t>
         </is>
       </c>
       <c r="C10" t="n">
@@ -746,7 +746,7 @@
         <v>-12227020</v>
       </c>
       <c r="H10" s="2" t="n">
-        <v>45767.431891083</v>
+        <v>45786.07619457495</v>
       </c>
     </row>
     <row r="11">
@@ -757,7 +757,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Giảm Safety Stock từ 0 → 0 và Reorder Point từ 2035 → 1831 để tiết kiệm chi phí.</t>
+          <t>Reduce Safety Stock from 0 → 0 and Reorder Point from 2035 → 1831 to save costs.</t>
         </is>
       </c>
       <c r="C11" t="n">
@@ -776,7 +776,7 @@
         <v>-8461440</v>
       </c>
       <c r="H11" s="2" t="n">
-        <v>45767.431891083</v>
+        <v>45786.07619457495</v>
       </c>
     </row>
   </sheetData>

</xml_diff>